<commit_message>
Sound  And Sprite Update
</commit_message>
<xml_diff>
--- a/BlueTeam/TeamBlue/Assets/Terasurware/ItemTable.xlsx
+++ b/BlueTeam/TeamBlue/Assets/Terasurware/ItemTable.xlsx
@@ -222,18 +222,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>Helmet1</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Helmet2</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Helmet3</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>발전카드(교역)</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -291,6 +279,18 @@
   </si>
   <si>
     <t>Recipe2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Helemet2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Helemet3</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Helemet1</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -644,8 +644,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="K20" sqref="K20"/>
+    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="K22" sqref="K22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -877,7 +877,7 @@
         <v>1201</v>
       </c>
       <c r="B7" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="C7" t="s">
         <v>22</v>
@@ -912,7 +912,7 @@
         <v>1202</v>
       </c>
       <c r="B8" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="C8" t="s">
         <v>22</v>
@@ -1079,7 +1079,7 @@
         <v>5</v>
       </c>
       <c r="K12" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.3">
@@ -1114,7 +1114,7 @@
         <v>5</v>
       </c>
       <c r="K13" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.3">
@@ -1149,7 +1149,7 @@
         <v>5</v>
       </c>
       <c r="K14" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.3">
@@ -1184,7 +1184,7 @@
         <v>40</v>
       </c>
       <c r="K15" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.3">
@@ -1219,7 +1219,7 @@
         <v>20</v>
       </c>
       <c r="K16" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.3">
@@ -1254,7 +1254,7 @@
         <v>20</v>
       </c>
       <c r="K17" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.3">
@@ -1289,7 +1289,7 @@
         <v>80</v>
       </c>
       <c r="K18" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.3">
@@ -1297,7 +1297,7 @@
         <v>1332</v>
       </c>
       <c r="B19" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="C19" t="s">
         <v>22</v>
@@ -1324,7 +1324,7 @@
         <v>60</v>
       </c>
       <c r="K19" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.3">
@@ -1332,7 +1332,7 @@
         <v>1333</v>
       </c>
       <c r="B20" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="C20" t="s">
         <v>22</v>
@@ -1359,7 +1359,7 @@
         <v>80</v>
       </c>
       <c r="K20" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.3">
@@ -1429,7 +1429,7 @@
         <v>5</v>
       </c>
       <c r="K22" t="s">
-        <v>51</v>
+        <v>68</v>
       </c>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.3">
@@ -1464,7 +1464,7 @@
         <v>5</v>
       </c>
       <c r="K23" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.3">
@@ -1534,7 +1534,7 @@
         <v>20</v>
       </c>
       <c r="K25" t="s">
-        <v>52</v>
+        <v>66</v>
       </c>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.3">
@@ -1569,7 +1569,7 @@
         <v>20</v>
       </c>
       <c r="K26" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.3">
@@ -1639,7 +1639,7 @@
         <v>60</v>
       </c>
       <c r="K28" t="s">
-        <v>53</v>
+        <v>67</v>
       </c>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.3">
@@ -1674,7 +1674,7 @@
         <v>80</v>
       </c>
       <c r="K29" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
item image 로드 수정
</commit_message>
<xml_diff>
--- a/BlueTeam/TeamBlue/Assets/Terasurware/ItemTable.xlsx
+++ b/BlueTeam/TeamBlue/Assets/Terasurware/ItemTable.xlsx
@@ -282,15 +282,15 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
+    <t>Helemet3</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Helemet1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>Helemet2</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Helemet3</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Helemet1</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -644,8 +644,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="K22" sqref="K22"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K28" sqref="K28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -1429,7 +1429,7 @@
         <v>5</v>
       </c>
       <c r="K22" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.3">
@@ -1534,7 +1534,7 @@
         <v>20</v>
       </c>
       <c r="K25" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.3">
@@ -1639,7 +1639,7 @@
         <v>60</v>
       </c>
       <c r="K28" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.3">

</xml_diff>